<commit_message>
Mejorar Home - Planeación Script3 - Formato HU
</commit_message>
<xml_diff>
--- a/DISTRIBUCION SPRINTS.xlsx
+++ b/DISTRIBUCION SPRINTS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\CICLO 3 - C#-2022-02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\equipo-84-xx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>SPRINT NRO 1.</t>
   </si>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -716,10 +716,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18" t="s">
-        <v>5</v>
-      </c>
+      <c r="D12" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="18"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
@@ -731,7 +731,9 @@
         <v>8</v>
       </c>
       <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
+      <c r="D13" s="19" t="s">
+        <v>5</v>
+      </c>
       <c r="E13" s="19"/>
       <c r="F13" s="20" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
DETAILS - DELETE - PLANEACION SPRINT4
</commit_message>
<xml_diff>
--- a/DISTRIBUCION SPRINTS.xlsx
+++ b/DISTRIBUCION SPRINTS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
   <si>
     <t>SPRINT NRO 1.</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Script SQL con el DDL de la Base de Datos</t>
   </si>
   <si>
-    <t>Capa de Datos</t>
-  </si>
-  <si>
     <t>Capa de Dominio</t>
   </si>
   <si>
@@ -81,6 +78,39 @@
   </si>
   <si>
     <t>Backend - Historias de Usuario</t>
+  </si>
+  <si>
+    <t>Capa de Persistencia</t>
+  </si>
+  <si>
+    <t>Capa de Presentación</t>
+  </si>
+  <si>
+    <t>Capa de Consola</t>
+  </si>
+  <si>
+    <t>Creación de la Solución</t>
+  </si>
+  <si>
+    <t>Código de los Frontend</t>
+  </si>
+  <si>
+    <t>Desarrollo Modulo Formador (Insetar-Editar-Eliminar-Consultar-Listar) - con almacenamiento en la BD</t>
+  </si>
+  <si>
+    <t>Desarrollo Modulo Tutor (Insetar-Editar-Eliminar-Consultar-Listar)  - con almacenamiento en la BD</t>
+  </si>
+  <si>
+    <t>Desarrollo Modulo Beneficiario (Insetar-Editar-Eliminar-Consultar-Listar)  - con almacenamiento en la BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vDesarrollo Modulo Formador (Insetar-Editar-Eliminar-Consultar-Listar)</t>
+  </si>
+  <si>
+    <t>Desarrollo Modulo Equpipos (Insetar-Editar-Eliminar-Consultar-Listar)  - con almacenamiento en la BD</t>
+  </si>
+  <si>
+    <t>Desarrollo Modulo Proyectos (Insetar-Editar-Eliminar-Consultar-Listar) - con almacenamiento en la BD</t>
   </si>
 </sst>
 </file>
@@ -125,25 +155,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -175,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -206,32 +236,36 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="distributed"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="distributed"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="distributed"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="distributed"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -551,21 +585,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -574,21 +608,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -597,15 +631,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+        <v>14</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
@@ -614,171 +648,319 @@
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
+      <c r="C5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
+        <v>15</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="B7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="B9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
-      <c r="B10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="B10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
-      <c r="B11" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="B11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>9</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="B12" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="20"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>10</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="16"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
+        <v>11</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="19"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
+        <v>12</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="19"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>13</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="19"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="7">
+        <v>14</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="7">
+        <v>15</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="7">
+        <v>16</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="7">
+        <v>17</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="7">
+        <v>18</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="7">
+        <v>19</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="7">
+        <v>20</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A24" s="7">
         <v>10</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="2"/>
+      <c r="B24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="2"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="2"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>